<commit_message>
Individual test results added to comparison_chart.xlsx
git-svn-id: http://pdfainspector.googlecode.com/svn/trunk@52 1783f179-91b5-6867-892f-c6e3ac0b0089
</commit_message>
<xml_diff>
--- a/testcases/comparison_chart.xlsx
+++ b/testcases/comparison_chart.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="13335" windowHeight="5100"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="13335" windowHeight="5100" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Comparison Chart" sheetId="1" r:id="rId1"/>
+    <sheet name="PAC" sheetId="2" r:id="rId2"/>
+    <sheet name="eGovmon" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="69">
   <si>
     <t>Document is marked as tagged</t>
   </si>
@@ -166,6 +166,63 @@
   </si>
   <si>
     <t>Tab follows Document Structure</t>
+  </si>
+  <si>
+    <t>PAC Evaluation Results</t>
+  </si>
+  <si>
+    <t>course_eval</t>
+  </si>
+  <si>
+    <t>iTextXmlToPdfExample</t>
+  </si>
+  <si>
+    <t>moby</t>
+  </si>
+  <si>
+    <t>newton</t>
+  </si>
+  <si>
+    <t>PDF-Test-Print-to-PDF</t>
+  </si>
+  <si>
+    <t>rnua</t>
+  </si>
+  <si>
+    <t>rnua-noforms</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>tables-tagged</t>
+  </si>
+  <si>
+    <t>tables-tagged-edited</t>
+  </si>
+  <si>
+    <t>tables-untagged</t>
+  </si>
+  <si>
+    <t>testdocument-forms</t>
+  </si>
+  <si>
+    <t>testdocument-images</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Total Failed Tests</t>
+  </si>
+  <si>
+    <t>Total Failed Tests (excluding !)</t>
   </si>
 </sst>
 </file>
@@ -209,10 +266,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -511,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -722,24 +785,1220 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+    <col min="10" max="10" width="11.85546875" customWidth="1"/>
+    <col min="11" max="12" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M12" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M13" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M14" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M15" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
+      <c r="A17" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <v>7</v>
+      </c>
+      <c r="G17">
+        <v>15</v>
+      </c>
+      <c r="H17">
+        <v>3</v>
+      </c>
+      <c r="I17">
+        <v>2</v>
+      </c>
+      <c r="J17">
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <v>7</v>
+      </c>
+      <c r="L17">
+        <v>2</v>
+      </c>
+      <c r="M17">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="14" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N2" s="3"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="3"/>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N4" s="3"/>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N5" s="3"/>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N6" s="3"/>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N7" s="3"/>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N8" s="3"/>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N9" s="3"/>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N10" s="3"/>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N11" s="3"/>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>3</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="K13">
+        <v>3</v>
+      </c>
+      <c r="L13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added test cases generated from msword / primopdf
git-svn-id: http://pdfainspector.googlecode.com/svn/trunk@53 1783f179-91b5-6867-892f-c6e3ac0b0089
</commit_message>
<xml_diff>
--- a/testcases/comparison_chart.xlsx
+++ b/testcases/comparison_chart.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="13335" windowHeight="5100" activeTab="2"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="13335" windowHeight="5100"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison Chart" sheetId="1" r:id="rId1"/>
     <sheet name="PAC" sheetId="2" r:id="rId2"/>
     <sheet name="eGovmon" sheetId="3" r:id="rId3"/>
+    <sheet name="Adobe Quick Check" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="75">
   <si>
     <t>Document is marked as tagged</t>
   </si>
@@ -223,6 +224,24 @@
   </si>
   <si>
     <t>Total Failed Tests (excluding !)</t>
+  </si>
+  <si>
+    <t>starbucks_textonly-msword</t>
+  </si>
+  <si>
+    <t>starbucks_textonly-primopdf</t>
+  </si>
+  <si>
+    <t>starbucks_imageonly-msword</t>
+  </si>
+  <si>
+    <t>starbucks_imageonly-primopdf</t>
+  </si>
+  <si>
+    <t>Total Failed Tests:</t>
+  </si>
+  <si>
+    <t>Criteria for the following evaluators:</t>
   </si>
 </sst>
 </file>
@@ -572,10 +591,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B19"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -588,192 +607,200 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="E4" t="s">
-        <v>44</v>
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D5" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>38</v>
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" t="s">
-        <v>45</v>
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
-        <v>47</v>
+        <v>6</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>7</v>
+      </c>
+      <c r="E11" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
-      <c r="B16" t="s">
+    <row r="18" spans="1:5">
+      <c r="B18" t="s">
         <v>24</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" t="s">
         <v>33</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
-      <c r="B17" t="s">
+    <row r="19" spans="1:5">
+      <c r="B19" t="s">
         <v>17</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C19" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
-      <c r="B18" t="s">
+    <row r="20" spans="1:5">
+      <c r="B20" t="s">
         <v>18</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
-      <c r="B19" t="s">
+    <row r="21" spans="1:5">
+      <c r="B21" t="s">
         <v>22</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C21" t="s">
         <v>26</v>
       </c>
-      <c r="E19" t="s">
+      <c r="E21" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
-      <c r="E20" t="s">
+    <row r="22" spans="1:5">
+      <c r="E22" t="s">
         <v>48</v>
       </c>
     </row>
@@ -785,7 +812,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M17"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
@@ -800,13 +827,13 @@
     <col min="5" max="5" width="12" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" customWidth="1"/>
     <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="11.85546875" customWidth="1"/>
-    <col min="11" max="12" width="12" customWidth="1"/>
+    <col min="8" max="12" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11.85546875" customWidth="1"/>
+    <col min="15" max="16" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:17">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -832,22 +859,34 @@
         <v>57</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -876,19 +915,31 @@
         <v>58</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
+      <c r="N2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -914,13 +965,13 @@
         <v>58</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>58</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>58</v>
@@ -928,8 +979,20 @@
       <c r="M3" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="N3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -955,22 +1018,34 @@
         <v>59</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>59</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>59</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1010,8 +1085,20 @@
       <c r="M5" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="6" spans="1:13">
+      <c r="N5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1040,19 +1127,31 @@
         <v>58</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="M6" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="1:13">
+      <c r="N6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1078,13 +1177,13 @@
         <v>58</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>60</v>
@@ -1092,8 +1191,20 @@
       <c r="M7" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="N7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1119,22 +1230,34 @@
         <v>58</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>60</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="M8" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="N8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1163,19 +1286,31 @@
         <v>58</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
+      <c r="N9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1201,22 +1336,34 @@
         <v>58</v>
       </c>
       <c r="I10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="J10" s="3" t="s">
+      <c r="N10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="K10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="M10" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="O10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1245,19 +1392,31 @@
         <v>58</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="M11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q11" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:13">
+    <row r="12" spans="1:17">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1286,19 +1445,31 @@
         <v>58</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="M12" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
+        <v>58</v>
+      </c>
+      <c r="N12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q12" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1327,19 +1498,31 @@
         <v>59</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M13" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="14" spans="1:13">
+      <c r="N13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="O13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q13" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1379,8 +1562,20 @@
       <c r="M14" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="15" spans="1:13">
+      <c r="N14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q14" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1420,8 +1615,20 @@
       <c r="M15" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="17" spans="1:13">
+      <c r="N15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q15" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" s="1" t="s">
         <v>68</v>
       </c>
@@ -1450,15 +1657,27 @@
         <v>2</v>
       </c>
       <c r="J17">
+        <v>7</v>
+      </c>
+      <c r="K17">
         <v>2</v>
       </c>
-      <c r="K17">
+      <c r="L17">
         <v>7</v>
       </c>
-      <c r="L17">
+      <c r="M17">
         <v>2</v>
       </c>
-      <c r="M17">
+      <c r="N17">
+        <v>2</v>
+      </c>
+      <c r="O17">
+        <v>7</v>
+      </c>
+      <c r="P17">
+        <v>2</v>
+      </c>
+      <c r="Q17">
         <v>2</v>
       </c>
     </row>
@@ -1469,19 +1688,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N13"/>
+  <dimension ref="A1:R13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:Q1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="14" width="11.7109375" customWidth="1"/>
+    <col min="2" max="18" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1491,7 +1710,7 @@
       <c r="C1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>53</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -1507,22 +1726,34 @@
         <v>57</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1551,20 +1782,32 @@
         <v>58</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="N2" s="3"/>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="N2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="R2" s="3"/>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1590,13 +1833,13 @@
         <v>58</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>58</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>58</v>
@@ -1604,9 +1847,21 @@
       <c r="M3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="N3" s="3"/>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="N3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="R3" s="3"/>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1632,23 +1887,35 @@
         <v>59</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>59</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N4" s="3"/>
-    </row>
-    <row r="5" spans="1:14">
+        <v>59</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="R4" s="3"/>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1688,9 +1955,21 @@
       <c r="M5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="N5" s="3"/>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="N5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="R5" s="3"/>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -1730,9 +2009,21 @@
       <c r="M6" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="N6" s="3"/>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="N6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="R6" s="3"/>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -1758,23 +2049,35 @@
         <v>58</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>59</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="M7" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="N7" s="3"/>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="N7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="R7" s="3"/>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1814,9 +2117,21 @@
       <c r="M8" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="N8" s="3"/>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="N8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="R8" s="3"/>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -1856,9 +2171,21 @@
       <c r="M9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="N9" s="3"/>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="N9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="R9" s="3"/>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -1887,20 +2214,32 @@
         <v>58</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>58</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="M10" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="N10" s="3"/>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="N10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="R10" s="3"/>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1935,14 +2274,26 @@
         <v>58</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="N11" s="3"/>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="N11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="R11" s="3"/>
+    </row>
+    <row r="12" spans="1:18">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -1951,13 +2302,17 @@
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
-      <c r="J12" s="4"/>
+      <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="N12" s="4"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="3"/>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" s="1" t="s">
         <v>67</v>
       </c>
@@ -1983,18 +2338,367 @@
         <v>2</v>
       </c>
       <c r="I13">
+        <v>2</v>
+      </c>
+      <c r="J13">
+        <v>4</v>
+      </c>
+      <c r="K13">
+        <v>2</v>
+      </c>
+      <c r="L13">
+        <v>4</v>
+      </c>
+      <c r="M13">
         <v>1</v>
       </c>
-      <c r="J13">
+      <c r="N13">
         <v>1</v>
       </c>
-      <c r="K13">
+      <c r="O13">
         <v>3</v>
       </c>
-      <c r="L13">
+      <c r="P13">
         <v>1</v>
       </c>
-      <c r="M13">
+      <c r="Q13">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:Q7"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="17" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>1</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding all xml files for anyone's reference.
git-svn-id: http://pdfainspector.googlecode.com/svn/trunk@66 1783f179-91b5-6867-892f-c6e3ac0b0089
</commit_message>
<xml_diff>
--- a/testcases/comparison_chart.xlsx
+++ b/testcases/comparison_chart.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="135" windowWidth="13335" windowHeight="5100"/>
+    <workbookView xWindow="480" yWindow="135" windowWidth="13335" windowHeight="5100" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Comparison Chart" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="80">
   <si>
     <t>Document is marked as tagged</t>
   </si>
@@ -242,6 +242,21 @@
   </si>
   <si>
     <t>Criteria for the following evaluators:</t>
+  </si>
+  <si>
+    <t>indesign-form</t>
+  </si>
+  <si>
+    <t>indesign-image</t>
+  </si>
+  <si>
+    <t>indesign-tables</t>
+  </si>
+  <si>
+    <t>indesign-textonly</t>
+  </si>
+  <si>
+    <t>indesign-forms</t>
   </si>
 </sst>
 </file>
@@ -593,7 +608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -812,28 +827,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q17"/>
+  <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.85546875" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" customWidth="1"/>
-    <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="8" max="12" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" customWidth="1"/>
-    <col min="14" max="14" width="11.85546875" customWidth="1"/>
-    <col min="15" max="16" width="12" customWidth="1"/>
+    <col min="2" max="6" width="12.42578125" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" customWidth="1"/>
+    <col min="12" max="16" width="12.85546875" customWidth="1"/>
+    <col min="17" max="17" width="11.7109375" customWidth="1"/>
+    <col min="18" max="18" width="11.85546875" customWidth="1"/>
+    <col min="19" max="20" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:21">
       <c r="A1" s="2" t="s">
         <v>50</v>
       </c>
@@ -841,52 +856,64 @@
         <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -894,52 +921,64 @@
         <v>59</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>58</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="L2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>58</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="R2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -953,37 +992,37 @@
         <v>59</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K3" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K3" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="L3" s="3" t="s">
         <v>58</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>58</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>58</v>
@@ -991,8 +1030,20 @@
       <c r="Q3" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="R3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1012,40 +1063,52 @@
         <v>59</v>
       </c>
       <c r="G4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="L4" s="3" t="s">
         <v>59</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>59</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+        <v>59</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1065,20 +1128,20 @@
         <v>58</v>
       </c>
       <c r="G5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K5" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="L5" s="3" t="s">
         <v>58</v>
       </c>
@@ -1097,8 +1160,20 @@
       <c r="Q5" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="6" spans="1:17">
+      <c r="R5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1118,20 +1193,20 @@
         <v>59</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="L6" s="3" t="s">
         <v>59</v>
       </c>
@@ -1139,19 +1214,31 @@
         <v>58</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q6" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="R6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1165,37 +1252,37 @@
         <v>60</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>60</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>60</v>
       </c>
       <c r="K7" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M7" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="M7" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N7" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="O7" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="P7" s="3" t="s">
         <v>60</v>
@@ -1203,8 +1290,20 @@
       <c r="Q7" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="8" spans="1:17">
+      <c r="R7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1224,10 +1323,10 @@
         <v>60</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>60</v>
@@ -1236,28 +1335,40 @@
         <v>60</v>
       </c>
       <c r="K8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="M8" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="N8" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="M8" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="N8" s="3" t="s">
-        <v>58</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>60</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="Q8" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="9" spans="1:17">
+      <c r="R8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1265,52 +1376,64 @@
         <v>59</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>58</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K9" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="L9" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M9" s="3" t="s">
         <v>58</v>
       </c>
       <c r="N9" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P9" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q9" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="10" spans="1:17">
+      <c r="R9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1318,52 +1441,64 @@
         <v>59</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>58</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K10" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K10" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="L10" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="N10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="N10" s="3" t="s">
+      <c r="R10" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="O10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q10" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17">
+      <c r="S10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1371,52 +1506,64 @@
         <v>59</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>58</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K11" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H11" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="L11" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M11" s="3" t="s">
         <v>58</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O11" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="R11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U11" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:21">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1424,52 +1571,64 @@
         <v>59</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K12" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H12" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J12" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="K12" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="L12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M12" s="3" t="s">
         <v>58</v>
       </c>
       <c r="N12" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P12" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q12" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17">
+        <v>58</v>
+      </c>
+      <c r="R12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="T12" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U12" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1477,52 +1636,64 @@
         <v>58</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K13" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H13" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="L13" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="M13" s="3" t="s">
         <v>59</v>
       </c>
       <c r="N13" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P13" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q13" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="14" spans="1:17">
+      <c r="R13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="S13" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="T13" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="U13" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
       <c r="A14" t="s">
         <v>39</v>
       </c>
@@ -1542,20 +1713,20 @@
         <v>58</v>
       </c>
       <c r="G14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K14" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H14" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I14" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J14" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="L14" s="3" t="s">
         <v>58</v>
       </c>
@@ -1574,8 +1745,20 @@
       <c r="Q14" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="15" spans="1:17">
+      <c r="R14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="T14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1595,20 +1778,20 @@
         <v>58</v>
       </c>
       <c r="G15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="K15" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I15" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J15" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="K15" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="L15" s="3" t="s">
         <v>58</v>
       </c>
@@ -1627,8 +1810,20 @@
       <c r="Q15" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="17" spans="1:17">
+      <c r="R15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="T15" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U15" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21">
       <c r="A17" s="1" t="s">
         <v>68</v>
       </c>
@@ -1636,48 +1831,60 @@
         <v>7</v>
       </c>
       <c r="C17">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D17">
         <v>4</v>
       </c>
       <c r="E17">
+        <v>4</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17">
+        <v>8</v>
+      </c>
+      <c r="H17">
+        <v>4</v>
+      </c>
+      <c r="I17">
         <v>7</v>
-      </c>
-      <c r="F17">
-        <v>7</v>
-      </c>
-      <c r="G17">
-        <v>15</v>
-      </c>
-      <c r="H17">
-        <v>3</v>
-      </c>
-      <c r="I17">
-        <v>2</v>
       </c>
       <c r="J17">
         <v>7</v>
       </c>
       <c r="K17">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="L17">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="M17">
         <v>2</v>
       </c>
       <c r="N17">
+        <v>7</v>
+      </c>
+      <c r="O17">
         <v>2</v>
       </c>
-      <c r="O17">
+      <c r="P17">
         <v>7</v>
       </c>
-      <c r="P17">
+      <c r="Q17">
         <v>2</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
+        <v>2</v>
+      </c>
+      <c r="S17">
+        <v>7</v>
+      </c>
+      <c r="T17">
+        <v>2</v>
+      </c>
+      <c r="U17">
         <v>2</v>
       </c>
     </row>
@@ -1688,19 +1895,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:R13"/>
+  <dimension ref="A1:V13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:Q1"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="18" width="11.7109375" customWidth="1"/>
+    <col min="2" max="22" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:22">
       <c r="A1" s="1" t="s">
         <v>13</v>
       </c>
@@ -1708,52 +1915,64 @@
         <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:18">
+    <row r="2" spans="1:22">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1761,25 +1980,25 @@
         <v>59</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>58</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>58</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>59</v>
@@ -1788,26 +2007,38 @@
         <v>58</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M2" s="3" t="s">
         <v>58</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="R2" s="3"/>
-    </row>
-    <row r="3" spans="1:18">
+      <c r="R2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="V2" s="3"/>
+    </row>
+    <row r="3" spans="1:22">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1821,37 +2052,37 @@
         <v>59</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J3" s="3" t="s">
         <v>58</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>58</v>
       </c>
       <c r="M3" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>58</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>58</v>
@@ -1859,9 +2090,21 @@
       <c r="Q3" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="R3" s="3"/>
-    </row>
-    <row r="4" spans="1:18">
+      <c r="R3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="V3" s="3"/>
+    </row>
+    <row r="4" spans="1:22">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -1887,35 +2130,47 @@
         <v>59</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>59</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>59</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>59</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="R4" s="3"/>
-    </row>
-    <row r="5" spans="1:18">
+        <v>59</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="V4" s="3"/>
+    </row>
+    <row r="5" spans="1:22">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1967,9 +2222,21 @@
       <c r="Q5" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="R5" s="3"/>
-    </row>
-    <row r="6" spans="1:18">
+      <c r="R5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="V5" s="3"/>
+    </row>
+    <row r="6" spans="1:22">
       <c r="A6" t="s">
         <v>19</v>
       </c>
@@ -2021,9 +2288,21 @@
       <c r="Q6" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="R6" s="3"/>
-    </row>
-    <row r="7" spans="1:18">
+      <c r="R6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="V6" s="3"/>
+    </row>
+    <row r="7" spans="1:22">
       <c r="A7" t="s">
         <v>21</v>
       </c>
@@ -2043,10 +2322,10 @@
         <v>59</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>59</v>
@@ -2055,29 +2334,41 @@
         <v>59</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>59</v>
       </c>
       <c r="P7" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q7" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="R7" s="3"/>
-    </row>
-    <row r="8" spans="1:18">
+      <c r="R7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="V7" s="3"/>
+    </row>
+    <row r="8" spans="1:22">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -2129,9 +2420,21 @@
       <c r="Q8" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="R8" s="3"/>
-    </row>
-    <row r="9" spans="1:18">
+      <c r="R8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U8" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="V8" s="3"/>
+    </row>
+    <row r="9" spans="1:22">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -2183,9 +2486,21 @@
       <c r="Q9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="R9" s="3"/>
-    </row>
-    <row r="10" spans="1:18">
+      <c r="R9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="T9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="V9" s="3"/>
+    </row>
+    <row r="10" spans="1:22">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -2205,19 +2520,19 @@
         <v>58</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>58</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>59</v>
@@ -2226,20 +2541,32 @@
         <v>58</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>58</v>
       </c>
       <c r="P10" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q10" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="R10" s="3"/>
-    </row>
-    <row r="11" spans="1:18">
+      <c r="R10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="T10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="V10" s="3"/>
+    </row>
+    <row r="11" spans="1:22">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -2259,7 +2586,7 @@
         <v>58</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>58</v>
@@ -2271,7 +2598,7 @@
         <v>58</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>58</v>
@@ -2286,14 +2613,26 @@
         <v>58</v>
       </c>
       <c r="P11" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q11" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="R11" s="3"/>
-    </row>
-    <row r="12" spans="1:18">
+      <c r="R11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="T11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="U11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="V11" s="3"/>
+    </row>
+    <row r="12" spans="1:22">
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -2306,13 +2645,17 @@
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
       <c r="M12" s="3"/>
-      <c r="N12" s="4"/>
+      <c r="N12" s="3"/>
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
       <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-    </row>
-    <row r="13" spans="1:18">
+      <c r="R12" s="4"/>
+      <c r="S12" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+      <c r="V12" s="3"/>
+    </row>
+    <row r="13" spans="1:22">
       <c r="A13" s="1" t="s">
         <v>67</v>
       </c>
@@ -2320,7 +2663,7 @@
         <v>3</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <v>3</v>
@@ -2332,36 +2675,48 @@
         <v>3</v>
       </c>
       <c r="G13">
+        <v>4</v>
+      </c>
+      <c r="H13">
         <v>3</v>
       </c>
-      <c r="H13">
+      <c r="I13">
+        <v>3</v>
+      </c>
+      <c r="J13">
+        <v>3</v>
+      </c>
+      <c r="K13">
+        <v>3</v>
+      </c>
+      <c r="L13">
         <v>2</v>
       </c>
-      <c r="I13">
+      <c r="M13">
         <v>2</v>
       </c>
-      <c r="J13">
+      <c r="N13">
         <v>4</v>
       </c>
-      <c r="K13">
+      <c r="O13">
         <v>2</v>
       </c>
-      <c r="L13">
+      <c r="P13">
         <v>4</v>
       </c>
-      <c r="M13">
+      <c r="Q13">
         <v>1</v>
       </c>
-      <c r="N13">
+      <c r="R13">
         <v>1</v>
       </c>
-      <c r="O13">
+      <c r="S13">
         <v>3</v>
       </c>
-      <c r="P13">
+      <c r="T13">
         <v>1</v>
       </c>
-      <c r="Q13">
+      <c r="U13">
         <v>0</v>
       </c>
     </row>
@@ -2372,19 +2727,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q7"/>
+  <dimension ref="A1:U7"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="17" width="11.7109375" customWidth="1"/>
+    <col min="2" max="21" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:21">
       <c r="A1" s="1" t="s">
         <v>42</v>
       </c>
@@ -2392,52 +2747,64 @@
         <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:21">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -2489,8 +2856,20 @@
       <c r="Q2" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="3" spans="1:17">
+      <c r="R2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
       <c r="A3" t="s">
         <v>36</v>
       </c>
@@ -2542,8 +2921,20 @@
       <c r="Q3" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="4" spans="1:17">
+      <c r="R3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -2551,25 +2942,25 @@
         <v>59</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>58</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>58</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>59</v>
@@ -2578,25 +2969,37 @@
         <v>58</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>58</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="Q4" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="5" spans="1:17">
+      <c r="R4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S4" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U4" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
       <c r="A5" t="s">
         <v>40</v>
       </c>
@@ -2648,8 +3051,20 @@
       <c r="Q5" s="3" t="s">
         <v>58</v>
       </c>
-    </row>
-    <row r="7" spans="1:17">
+      <c r="R5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="S5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="U5" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
       <c r="A7" s="1" t="s">
         <v>73</v>
       </c>
@@ -2657,25 +3072,25 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
         <v>1</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
       <c r="I7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -2684,21 +3099,33 @@
         <v>0</v>
       </c>
       <c r="L7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M7">
         <v>0</v>
       </c>
       <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
         <v>0</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <v>1</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <v>0</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7">
+        <v>1</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
         <v>0</v>
       </c>
     </row>

</xml_diff>